<commit_message>
Update LuckySpinSimulator -  tools
</commit_message>
<xml_diff>
--- a/LuckySpin/LuckySpinSystem.xlsx
+++ b/LuckySpin/LuckySpinSystem.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanxin/Gamedev_Tools/LuckySpin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD601B15-78FF-9F43-86F4-3151B133005B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD84DC4-1FD7-2B40-801B-A288E83AE240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{CB3C4474-0FCA-FB4A-8237-8B08E4EA6766}"/>
+    <workbookView xWindow="-2840" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{CB3C4474-0FCA-FB4A-8237-8B08E4EA6766}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="思路1" sheetId="1" r:id="rId1"/>
+    <sheet name="思路1数据" sheetId="2" r:id="rId2"/>
+    <sheet name="整理" sheetId="3" r:id="rId3"/>
+    <sheet name="8BALL" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="157">
   <si>
     <t>SPin items</t>
   </si>
@@ -414,6 +416,99 @@
   </si>
   <si>
     <t>台球不同层级玩家所转次数的分布</t>
+  </si>
+  <si>
+    <t xml:space="preserve">数据 &amp; 模型 </t>
+  </si>
+  <si>
+    <t>价值比例</t>
+  </si>
+  <si>
+    <t>水晶球*28</t>
+  </si>
+  <si>
+    <t>瓦吉特*6</t>
+  </si>
+  <si>
+    <t>消耗品*2</t>
+  </si>
+  <si>
+    <t>审判*1</t>
+  </si>
+  <si>
+    <t>钻石*200</t>
+  </si>
+  <si>
+    <t>钻石*20</t>
+  </si>
+  <si>
+    <t>花岗岩*130</t>
+  </si>
+  <si>
+    <t>金币*800</t>
+  </si>
+  <si>
+    <t>次数</t>
+  </si>
+  <si>
+    <t>消耗</t>
+  </si>
+  <si>
+    <t>获得</t>
+  </si>
+  <si>
+    <t>金币*1000</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>触发广告</t>
+  </si>
+  <si>
+    <t>金币*2000</t>
+  </si>
+  <si>
+    <t>金币*4000</t>
+  </si>
+  <si>
+    <t>金币*6000</t>
+  </si>
+  <si>
+    <t>价值体系</t>
+  </si>
+  <si>
+    <t>金币*9000</t>
+  </si>
+  <si>
+    <t>金币*12000</t>
+  </si>
+  <si>
+    <t>金币*16000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>与GOLFRIVAL一致</t>
+  </si>
+  <si>
+    <t>特定紫卡</t>
+  </si>
+  <si>
+    <t>40万能/80特定</t>
+  </si>
+  <si>
+    <t>设计期望次数</t>
+  </si>
+  <si>
+    <t>随机紫卡/随机橙卡</t>
+  </si>
+  <si>
+    <t>钻石 *20</t>
+  </si>
+  <si>
+    <t>20💎</t>
   </si>
 </sst>
 </file>
@@ -456,7 +551,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +588,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -522,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -539,6 +646,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,7 +761,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$18:$L$18</c:f>
+              <c:f>思路1!$E$18:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2667,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C35C7-C6FC-2F46-970F-3FAF8E8F73EA}">
-  <dimension ref="A1:AC103"/>
+  <dimension ref="A1:AC116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3286,16 +3398,16 @@
         <f>60/1000</f>
         <v>0.06</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
       <c r="M16" t="s">
         <v>20</v>
       </c>
@@ -4572,6 +4684,11 @@
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4588,7 +4705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFE4735-F306-9246-8E01-EF29E009A6A5}">
   <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="110" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="110" workbookViewId="0">
       <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
@@ -4999,4 +5116,1429 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57362D8D-9DE4-3941-8D7C-F497254A6CFE}">
+  <dimension ref="A1:AD38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="39.1640625" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <f>40*B27</f>
+        <v>1240</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1">
+        <v>50</v>
+      </c>
+      <c r="M4" s="1">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1">
+        <v>7.0489493676683628</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <f>D5*A16</f>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>400</v>
+      </c>
+      <c r="F5" s="1">
+        <v>500</v>
+      </c>
+      <c r="G5" s="1">
+        <v>600</v>
+      </c>
+      <c r="H5" s="1">
+        <v>700</v>
+      </c>
+      <c r="I5" s="1">
+        <v>800</v>
+      </c>
+      <c r="J5" s="1">
+        <v>900</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1100</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3.4062586252690648</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1">
+        <v>150</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1">
+        <v>250</v>
+      </c>
+      <c r="I6" s="1">
+        <v>300</v>
+      </c>
+      <c r="J6" s="1">
+        <v>350</v>
+      </c>
+      <c r="K6" s="1">
+        <v>400</v>
+      </c>
+      <c r="L6" s="1">
+        <v>450</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5.3868643289317895</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="1">
+        <v>200</v>
+      </c>
+      <c r="F7" s="1">
+        <v>250</v>
+      </c>
+      <c r="G7" s="1">
+        <v>300</v>
+      </c>
+      <c r="H7" s="1">
+        <v>350</v>
+      </c>
+      <c r="I7" s="1">
+        <v>400</v>
+      </c>
+      <c r="J7" s="1">
+        <v>450</v>
+      </c>
+      <c r="K7" s="1">
+        <v>500</v>
+      </c>
+      <c r="L7" s="1">
+        <v>550</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4</v>
+      </c>
+      <c r="N7" s="1">
+        <v>4.65081715690898</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="1">
+        <v>200</v>
+      </c>
+      <c r="F8" s="1">
+        <v>250</v>
+      </c>
+      <c r="G8" s="1">
+        <v>300</v>
+      </c>
+      <c r="H8" s="1">
+        <v>350</v>
+      </c>
+      <c r="I8" s="1">
+        <v>400</v>
+      </c>
+      <c r="J8" s="1">
+        <v>450</v>
+      </c>
+      <c r="K8" s="1">
+        <v>500</v>
+      </c>
+      <c r="L8" s="1">
+        <v>550</v>
+      </c>
+      <c r="M8" s="1">
+        <v>6</v>
+      </c>
+      <c r="N8" s="1">
+        <v>4.6508171569089667</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <f>300*A16</f>
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="1">
+        <v>300</v>
+      </c>
+      <c r="E9" s="1">
+        <v>500</v>
+      </c>
+      <c r="F9" s="1">
+        <v>600</v>
+      </c>
+      <c r="G9" s="1">
+        <v>700</v>
+      </c>
+      <c r="H9" s="1">
+        <v>800</v>
+      </c>
+      <c r="I9" s="1">
+        <v>900</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1100</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1200</v>
+      </c>
+      <c r="M9" s="1">
+        <v>7</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3.102738103701975</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="1">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1">
+        <v>250</v>
+      </c>
+      <c r="G10" s="1">
+        <v>300</v>
+      </c>
+      <c r="H10" s="1">
+        <v>350</v>
+      </c>
+      <c r="I10" s="1">
+        <v>400</v>
+      </c>
+      <c r="J10" s="1">
+        <v>450</v>
+      </c>
+      <c r="K10" s="1">
+        <v>500</v>
+      </c>
+      <c r="L10" s="1">
+        <v>550</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1">
+        <v>4.6508171569089471</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <f>500*A16</f>
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="1">
+        <v>500</v>
+      </c>
+      <c r="E11" s="1">
+        <v>500</v>
+      </c>
+      <c r="F11" s="1">
+        <v>600</v>
+      </c>
+      <c r="G11" s="1">
+        <v>700</v>
+      </c>
+      <c r="H11" s="1">
+        <v>800</v>
+      </c>
+      <c r="I11" s="1">
+        <v>900</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1100</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1200</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3.102738103701943</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B4:B11)</f>
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f>60/1000</f>
+        <v>0.06</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="13"/>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f>60/(1000*1.3)</f>
+        <v>4.6153846153846156E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18">
+        <v>400</v>
+      </c>
+      <c r="H18">
+        <v>600</v>
+      </c>
+      <c r="I18">
+        <v>600</v>
+      </c>
+      <c r="J18">
+        <v>1000</v>
+      </c>
+      <c r="K18">
+        <v>1500</v>
+      </c>
+      <c r="L18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19">
+        <f>E18*$A$18</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19:L19" si="0">F18*$A$18</f>
+        <v>9.2307692307692317</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>18.461538461538463</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>27.692307692307693</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>27.692307692307693</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>46.153846153846153</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>69.230769230769241</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>92.307692307692307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20">
+        <f>SUM($E$19:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>SUM($E$19:F19)</f>
+        <v>9.2307692307692317</v>
+      </c>
+      <c r="G20">
+        <f>SUM($E$19:G19)</f>
+        <v>27.692307692307693</v>
+      </c>
+      <c r="H20">
+        <f>SUM($E$19:H19)</f>
+        <v>55.384615384615387</v>
+      </c>
+      <c r="I20">
+        <f>SUM($E$19:I19)</f>
+        <v>83.07692307692308</v>
+      </c>
+      <c r="J20">
+        <f>SUM($E$19:J19)</f>
+        <v>129.23076923076923</v>
+      </c>
+      <c r="K20">
+        <f>SUM($E$19:K19)</f>
+        <v>198.46153846153845</v>
+      </c>
+      <c r="L20">
+        <f>SUM($E$19:L19)</f>
+        <v>290.76923076923077</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I21" s="12"/>
+      <c r="J21" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="12">
+        <f>SUM(I19:L19)</f>
+        <v>235.38461538461542</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22">
+        <f>E18*$A$16</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:L22" si="1">F18*$A$16</f>
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="O22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23">
+        <f>SUM($E$22:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>SUM($E$22:F22)</f>
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <f>SUM($E$22:G22)</f>
+        <v>36</v>
+      </c>
+      <c r="H23">
+        <f>SUM($E$22:H22)</f>
+        <v>72</v>
+      </c>
+      <c r="I23">
+        <f>SUM($E$22:I22)</f>
+        <v>108</v>
+      </c>
+      <c r="J23">
+        <f>SUM($E$22:J22)</f>
+        <v>168</v>
+      </c>
+      <c r="K23">
+        <f>SUM($E$22:K22)</f>
+        <v>258</v>
+      </c>
+      <c r="L23">
+        <f>SUM($E$22:L22)</f>
+        <v>378</v>
+      </c>
+      <c r="O23">
+        <f>B12/L23</f>
+        <v>3.925925925925926</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27">
+        <f>2790/90</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <f>1440/90</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <f>(E4/(SUM(E$4:E$11))*$B4)</f>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:L29" si="2">(F4/(SUM(F$4:F$11))*$B4)</f>
+        <v>2.3800383877159308</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>3.987138263665595</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>5.1452282157676352</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>6.0194174757281544</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>8.0345572354211665</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>9.6498054474708166</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>10.973451327433628</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <f t="shared" ref="E30:L36" si="3">(E5/(SUM(E$4:E$11))*$B5)</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>1.1516314779270633</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>1.157556270096463</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>1.1618257261410789</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>1.1650485436893203</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>1.1663066954643628</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>1.1673151750972763</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>1.168141592920354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>1.4285714285714284</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>1.727447216890595</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>1.9292604501607715</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>2.0746887966804981</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>2.1844660194174756</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>2.2678185745140391</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>2.3346303501945527</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="3"/>
+        <v>2.3893805309734515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>4.7619047619047619</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>4.7984644913627639</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>4.823151125401929</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>4.8409405255878291</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>4.8543689320388346</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>4.8596112311015123</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>4.8638132295719849</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="3"/>
+        <v>4.8672566371681416</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>5.7142857142857135</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>5.7581573896353166</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>5.787781350482315</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>5.809128630705394</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>5.825242718446602</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>5.8315334773218144</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>5.836575875486381</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="3"/>
+        <v>5.8407079646017701</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>4.1458733205374285</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>4.051446945337621</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>3.9834024896265561</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>3.9320388349514559</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>3.8876889848812093</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>3.8521400778210113</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>3.8230088495575218</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>4.7619047619047619</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>4.7984644913627639</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>4.823151125401929</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>4.8409405255878291</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>4.8543689320388346</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>4.8596112311015123</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>4.8638132295719849</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="3"/>
+        <v>4.8672566371681416</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>6.90978886756238</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>6.752411575562701</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>6.6390041493775929</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>6.5533980582524265</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>6.4794816414686824</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>6.4202334630350189</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="3"/>
+        <v>6.3716814159292037</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <f>SUM(E29:E36)</f>
+        <v>29.238095238095237</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ref="F38:L38" si="4">SUM(F29:F36)</f>
+        <v>31.669865642994242</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>33.311897106109328</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>34.49515905947441</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>35.388349514563103</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="4"/>
+        <v>37.386609071274293</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="4"/>
+        <v>38.988326848249031</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="4"/>
+        <v>40.30088495575221</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E16:L16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A634A7-831D-7840-8E63-AE9E936DC34A}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>